<commit_message>
Fixed error in input calculations
</commit_message>
<xml_diff>
--- a/New code/Inputs.xlsx
+++ b/New code/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\NREL\PVTesBattery\New code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA60B29D-332B-4046-AAB5-2A9CE5C9A600}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F846403-06E6-49E6-A2D1-5ECE8275EE57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{058D1A83-AC5B-4028-8283-EEC5B882409C}"/>
+    <workbookView xWindow="5190" yWindow="3810" windowWidth="21600" windowHeight="11385" xr2:uid="{058D1A83-AC5B-4028-8283-EEC5B882409C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,8 +568,8 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>B4/B5</f>
-        <v>100</v>
+        <f>B5/B3</f>
+        <v>32.594524119947849</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>